<commit_message>
Improved WLESS_SendPacketBurst's transmission time to nearly 3 times faster.
</commit_message>
<xml_diff>
--- a/WirelessTimingData.xlsx
+++ b/WirelessTimingData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\campus.mcgill.ca\emf\CPE\kcadie1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\microp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Start Time (s)</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>10 2byte burst FEC + DW</t>
+  </si>
+  <si>
+    <t>10 2-byte burst FEC + DW + Improved transmission method</t>
+  </si>
+  <si>
+    <t>Frequency (Hz)</t>
   </si>
 </sst>
 </file>
@@ -368,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:I28"/>
+  <dimension ref="B4:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,6 +389,7 @@
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -602,8 +609,18 @@
         <f t="shared" si="0"/>
         <v>1.4223700000002282</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>4.0006612500000003</v>
+      </c>
+      <c r="H16">
+        <v>4.0128336100000004</v>
+      </c>
+      <c r="I16">
+        <f>(H16-G16)*1000</f>
+        <v>12.172360000000104</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>11</v>
       </c>
@@ -618,7 +635,7 @@
         <v>1.4250300000000493</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>12</v>
       </c>
@@ -633,7 +650,7 @@
         <v>1.4256100000000771</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>13</v>
       </c>
@@ -647,8 +664,14 @@
         <f t="shared" si="0"/>
         <v>1.4256200000000163</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>14</v>
       </c>
@@ -662,8 +685,22 @@
         <f t="shared" si="0"/>
         <v>1.4254299999993947</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>4.00066364</v>
+      </c>
+      <c r="H20">
+        <v>4.0051203299999996</v>
+      </c>
+      <c r="I20">
+        <f>(H20-G20)*1000</f>
+        <v>4.4566899999995968</v>
+      </c>
+      <c r="L20">
+        <f>1000/I20</f>
+        <v>224.38177212238017</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>15</v>
       </c>
@@ -678,7 +715,7 @@
         <v>1.4223800000001674</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>16</v>
       </c>
@@ -693,7 +730,7 @@
         <v>1.4254899999999182</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>17</v>
       </c>
@@ -708,7 +745,7 @@
         <v>1.4223500000003497</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>18</v>
       </c>
@@ -723,7 +760,7 @@
         <v>1.422199999999485</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>19</v>
       </c>
@@ -738,7 +775,7 @@
         <v>1.4221700000005555</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>20</v>
       </c>
@@ -753,7 +790,7 @@
         <v>1.422789999999452</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>4</v>
       </c>

</xml_diff>